<commit_message>
tablas desc y corr
</commit_message>
<xml_diff>
--- a/3_output/tablas/test_hipotesis.xlsx
+++ b/3_output/tablas/test_hipotesis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\OneDrive - Universidad Católica de Chile\Investigación y proyectos\[COBA] Cohesión Barrial\dse-cob-tesis\3_output\tablas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/ciortiz1_uc_cl/Documents/Investigación y proyectos/[COBA] Cohesión Barrial/dse-cob-tesis/3_output/tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321BA113-D5C5-4DAA-BA7B-EF9557309899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{321BA113-D5C5-4DAA-BA7B-EF9557309899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67C420A4-B41D-44B9-BB99-3AC981C1EF25}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="16305" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="887" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="formulación" sheetId="11" r:id="rId1"/>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8EB2B2-57D8-406B-8019-952C42E865B7}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,16 +756,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F74542-A909-4FCA-94EB-1CB54FFD1CD8}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6328125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" customWidth="1"/>
     <col min="2" max="2" width="35.7265625" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>